<commit_message>
Correcion de error en exportacion
</commit_message>
<xml_diff>
--- a/Spa Diego/SpaDiego_Analisis/Archivos resultados/CLIENTE TODO SERVICIO.xlsx
+++ b/Spa Diego/SpaDiego_Analisis/Archivos resultados/CLIENTE TODO SERVICIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alexander\Documents\GitHub\Desafio1_DMD\Spa Diego\SpaDiego_Analisis\Archivos resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0731CF49-D19B-4B51-875B-996C3CDAC67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26470778-550E-4302-B0AE-39A87CDE9854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Nombre Cliente</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>Utiliza Yoga</t>
+  </si>
+  <si>
+    <t>Edad</t>
   </si>
 </sst>
 </file>
@@ -405,53 +408,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="16.85546875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" style="5" customWidth="1"/>
-    <col min="5" max="9" width="16.85546875" customWidth="1"/>
+    <col min="1" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" style="3" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="5" customWidth="1"/>
+    <col min="6" max="10" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row spans="1:9" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row spans="1:10" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row outlineLevel="0" r="2">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>JOBI MCINTEE</t>
+          <t>AME CRUM</t>
         </is>
       </c>
       <c r="B2" s="0" t="inlineStr">
@@ -461,22 +467,22 @@
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>543.21000000000004</t>
+          <t>30</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>3.6499999999999999</t>
+          <t>2999.1999999999998</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3.2799999999999998</t>
         </is>
       </c>
       <c r="F2" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G2" s="0" t="inlineStr">
@@ -490,6 +496,11 @@
         </is>
       </c>
       <c r="I2" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J2" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -498,7 +509,7 @@
     <row outlineLevel="0" r="3">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>DOROTEYA ROOKEBY</t>
+          <t>ANSTICE DRACHE</t>
         </is>
       </c>
       <c r="B3" s="0" t="inlineStr">
@@ -508,22 +519,22 @@
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>597.66999999999996</t>
+          <t>49</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>1.6100000000000001</t>
+          <t>2916.96</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2.5699999999999998</t>
         </is>
       </c>
       <c r="F3" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G3" s="0" t="inlineStr">
@@ -537,6 +548,11 @@
         </is>
       </c>
       <c r="I3" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J3" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -545,32 +561,32 @@
     <row outlineLevel="0" r="4">
       <c r="A4" s="0" t="inlineStr">
         <is>
-          <t>MARCHELLE WITHROP</t>
+          <t>BEVVY CARRAGHER</t>
         </is>
       </c>
       <c r="B4" s="0" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C4" s="0" t="inlineStr">
         <is>
-          <t>663.26999999999998</t>
+          <t>34</t>
         </is>
       </c>
       <c r="D4" s="0" t="inlineStr">
         <is>
-          <t>1.27</t>
+          <t>2875.3499999999999</t>
         </is>
       </c>
       <c r="E4" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>2.3399999999999999</t>
         </is>
       </c>
       <c r="F4" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G4" s="0" t="inlineStr">
@@ -584,6 +600,11 @@
         </is>
       </c>
       <c r="I4" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J4" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -592,32 +613,32 @@
     <row outlineLevel="0" r="5">
       <c r="A5" s="0" t="inlineStr">
         <is>
-          <t>TRIS DOCHON</t>
+          <t>CAREY BILLINGTON</t>
         </is>
       </c>
       <c r="B5" s="0" t="inlineStr">
         <is>
-          <t>Hombre</t>
+          <t>Mujer</t>
         </is>
       </c>
       <c r="C5" s="0" t="inlineStr">
         <is>
-          <t>817.49000000000001</t>
+          <t>25</t>
         </is>
       </c>
       <c r="D5" s="0" t="inlineStr">
         <is>
-          <t>6.1100000000000003</t>
+          <t>2454.9400000000001</t>
         </is>
       </c>
       <c r="E5" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3.27</t>
         </is>
       </c>
       <c r="F5" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G5" s="0" t="inlineStr">
@@ -631,6 +652,11 @@
         </is>
       </c>
       <c r="I5" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J5" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -639,7 +665,7 @@
     <row outlineLevel="0" r="6">
       <c r="A6" s="0" t="inlineStr">
         <is>
-          <t>PIP WILFINGER</t>
+          <t>RENADO DOBIE</t>
         </is>
       </c>
       <c r="B6" s="0" t="inlineStr">
@@ -649,22 +675,22 @@
       </c>
       <c r="C6" s="0" t="inlineStr">
         <is>
-          <t>818.07000000000005</t>
+          <t>50</t>
         </is>
       </c>
       <c r="D6" s="0" t="inlineStr">
         <is>
-          <t>4.6200000000000001</t>
+          <t>2449.9400000000001</t>
         </is>
       </c>
       <c r="E6" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5.25</t>
         </is>
       </c>
       <c r="F6" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G6" s="0" t="inlineStr">
@@ -678,6 +704,11 @@
         </is>
       </c>
       <c r="I6" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J6" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -686,7 +717,7 @@
     <row outlineLevel="0" r="7">
       <c r="A7" s="0" t="inlineStr">
         <is>
-          <t>NELLI JAKES</t>
+          <t>JUNIE BLOWFIELD</t>
         </is>
       </c>
       <c r="B7" s="0" t="inlineStr">
@@ -696,22 +727,22 @@
       </c>
       <c r="C7" s="0" t="inlineStr">
         <is>
-          <t>821.05999999999995</t>
+          <t>38</t>
         </is>
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>5.1200000000000001</t>
+          <t>2448.2600000000002</t>
         </is>
       </c>
       <c r="E7" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.0800000000000001</t>
         </is>
       </c>
       <c r="F7" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G7" s="0" t="inlineStr">
@@ -725,6 +756,11 @@
         </is>
       </c>
       <c r="I7" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J7" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -733,7 +769,7 @@
     <row outlineLevel="0" r="8">
       <c r="A8" s="0" t="inlineStr">
         <is>
-          <t>ERWIN FOXWELL</t>
+          <t>ISA WAYMAN</t>
         </is>
       </c>
       <c r="B8" s="0" t="inlineStr">
@@ -743,22 +779,22 @@
       </c>
       <c r="C8" s="0" t="inlineStr">
         <is>
-          <t>849.94000000000005</t>
+          <t>54</t>
         </is>
       </c>
       <c r="D8" s="0" t="inlineStr">
         <is>
-          <t>4.2800000000000002</t>
+          <t>2415.1199999999999</t>
         </is>
       </c>
       <c r="E8" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5.4100000000000001</t>
         </is>
       </c>
       <c r="F8" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G8" s="0" t="inlineStr">
@@ -772,6 +808,11 @@
         </is>
       </c>
       <c r="I8" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J8" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -780,32 +821,32 @@
     <row outlineLevel="0" r="9">
       <c r="A9" s="0" t="inlineStr">
         <is>
-          <t>HUGHIE MARVELL</t>
+          <t>TREVER DU FRAY</t>
         </is>
       </c>
       <c r="B9" s="0" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C9" s="0" t="inlineStr">
         <is>
-          <t>954.70000000000005</t>
+          <t>45</t>
         </is>
       </c>
       <c r="D9" s="0" t="inlineStr">
         <is>
-          <t>3.9399999999999999</t>
+          <t>1937.0599999999999</t>
         </is>
       </c>
       <c r="E9" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6.7000000000000002</t>
         </is>
       </c>
       <c r="F9" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G9" s="0" t="inlineStr">
@@ -819,6 +860,11 @@
         </is>
       </c>
       <c r="I9" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J9" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -827,7 +873,7 @@
     <row outlineLevel="0" r="10">
       <c r="A10" s="0" t="inlineStr">
         <is>
-          <t>DAMITA BAELDE</t>
+          <t>ISSIAH LOB</t>
         </is>
       </c>
       <c r="B10" s="0" t="inlineStr">
@@ -837,22 +883,22 @@
       </c>
       <c r="C10" s="0" t="inlineStr">
         <is>
-          <t>1070.9200000000001</t>
+          <t>65</t>
         </is>
       </c>
       <c r="D10" s="0" t="inlineStr">
         <is>
-          <t>1.05</t>
+          <t>1923.3800000000001</t>
         </is>
       </c>
       <c r="E10" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5.3600000000000003</t>
         </is>
       </c>
       <c r="F10" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G10" s="0" t="inlineStr">
@@ -866,6 +912,11 @@
         </is>
       </c>
       <c r="I10" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J10" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -874,7 +925,7 @@
     <row outlineLevel="0" r="11">
       <c r="A11" s="0" t="inlineStr">
         <is>
-          <t>JEAN KILGANNON</t>
+          <t>ELEANORE CARELESS</t>
         </is>
       </c>
       <c r="B11" s="0" t="inlineStr">
@@ -884,22 +935,22 @@
       </c>
       <c r="C11" s="0" t="inlineStr">
         <is>
-          <t>1121.6099999999999</t>
+          <t>55</t>
         </is>
       </c>
       <c r="D11" s="0" t="inlineStr">
         <is>
-          <t>3.9900000000000002</t>
+          <t>1899.79</t>
         </is>
       </c>
       <c r="E11" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6.1699999999999999</t>
         </is>
       </c>
       <c r="F11" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G11" s="0" t="inlineStr">
@@ -913,6 +964,11 @@
         </is>
       </c>
       <c r="I11" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J11" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -921,7 +977,7 @@
     <row outlineLevel="0" r="12">
       <c r="A12" s="0" t="inlineStr">
         <is>
-          <t>DARNELL DINE-HART</t>
+          <t>ARNALDO BARENSEN</t>
         </is>
       </c>
       <c r="B12" s="0" t="inlineStr">
@@ -931,22 +987,22 @@
       </c>
       <c r="C12" s="0" t="inlineStr">
         <is>
-          <t>1307.02</t>
+          <t>61</t>
         </is>
       </c>
       <c r="D12" s="0" t="inlineStr">
         <is>
-          <t>3.1699999999999999</t>
+          <t>1868.46</t>
         </is>
       </c>
       <c r="E12" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.5499999999999998</t>
         </is>
       </c>
       <c r="F12" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G12" s="0" t="inlineStr">
@@ -960,6 +1016,11 @@
         </is>
       </c>
       <c r="I12" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J12" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -968,32 +1029,32 @@
     <row outlineLevel="0" r="13">
       <c r="A13" s="0" t="inlineStr">
         <is>
-          <t>MARCY BAKSTER</t>
+          <t>WOOD LE FLEMING</t>
         </is>
       </c>
       <c r="B13" s="0" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C13" s="0" t="inlineStr">
         <is>
-          <t>1418.1400000000001</t>
+          <t>42</t>
         </is>
       </c>
       <c r="D13" s="0" t="inlineStr">
         <is>
-          <t>6.5</t>
+          <t>1687.03</t>
         </is>
       </c>
       <c r="E13" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.7400000000000002</t>
         </is>
       </c>
       <c r="F13" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G13" s="0" t="inlineStr">
@@ -1007,6 +1068,11 @@
         </is>
       </c>
       <c r="I13" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J13" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1015,7 +1081,7 @@
     <row outlineLevel="0" r="14">
       <c r="A14" s="0" t="inlineStr">
         <is>
-          <t>BENDICK KOBIELA</t>
+          <t>PERSIS LOIDL</t>
         </is>
       </c>
       <c r="B14" s="0" t="inlineStr">
@@ -1025,22 +1091,22 @@
       </c>
       <c r="C14" s="0" t="inlineStr">
         <is>
-          <t>1570.3299999999999</t>
+          <t>58</t>
         </is>
       </c>
       <c r="D14" s="0" t="inlineStr">
         <is>
-          <t>4.9500000000000002</t>
+          <t>1620.7</t>
         </is>
       </c>
       <c r="E14" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.8600000000000001</t>
         </is>
       </c>
       <c r="F14" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G14" s="0" t="inlineStr">
@@ -1054,6 +1120,11 @@
         </is>
       </c>
       <c r="I14" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J14" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1062,7 +1133,7 @@
     <row outlineLevel="0" r="15">
       <c r="A15" s="0" t="inlineStr">
         <is>
-          <t>PERSIS LOIDL</t>
+          <t>BENDICK KOBIELA</t>
         </is>
       </c>
       <c r="B15" s="0" t="inlineStr">
@@ -1072,22 +1143,22 @@
       </c>
       <c r="C15" s="0" t="inlineStr">
         <is>
-          <t>1620.7</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D15" s="0" t="inlineStr">
         <is>
-          <t>1.8600000000000001</t>
+          <t>1570.3299999999999</t>
         </is>
       </c>
       <c r="E15" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.9500000000000002</t>
         </is>
       </c>
       <c r="F15" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G15" s="0" t="inlineStr">
@@ -1101,6 +1172,11 @@
         </is>
       </c>
       <c r="I15" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J15" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1109,32 +1185,32 @@
     <row outlineLevel="0" r="16">
       <c r="A16" s="0" t="inlineStr">
         <is>
-          <t>WOOD LE FLEMING</t>
+          <t>MARCY BAKSTER</t>
         </is>
       </c>
       <c r="B16" s="0" t="inlineStr">
         <is>
-          <t>Hombre</t>
+          <t>Mujer</t>
         </is>
       </c>
       <c r="C16" s="0" t="inlineStr">
         <is>
-          <t>1687.03</t>
+          <t>26</t>
         </is>
       </c>
       <c r="D16" s="0" t="inlineStr">
         <is>
-          <t>4.7400000000000002</t>
+          <t>1418.1400000000001</t>
         </is>
       </c>
       <c r="E16" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6.5</t>
         </is>
       </c>
       <c r="F16" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G16" s="0" t="inlineStr">
@@ -1148,6 +1224,11 @@
         </is>
       </c>
       <c r="I16" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J16" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1156,7 +1237,7 @@
     <row outlineLevel="0" r="17">
       <c r="A17" s="0" t="inlineStr">
         <is>
-          <t>ARNALDO BARENSEN</t>
+          <t>DARNELL DINE-HART</t>
         </is>
       </c>
       <c r="B17" s="0" t="inlineStr">
@@ -1166,22 +1247,22 @@
       </c>
       <c r="C17" s="0" t="inlineStr">
         <is>
-          <t>1868.46</t>
+          <t>63</t>
         </is>
       </c>
       <c r="D17" s="0" t="inlineStr">
         <is>
-          <t>4.5499999999999998</t>
+          <t>1307.02</t>
         </is>
       </c>
       <c r="E17" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3.1699999999999999</t>
         </is>
       </c>
       <c r="F17" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G17" s="0" t="inlineStr">
@@ -1195,6 +1276,11 @@
         </is>
       </c>
       <c r="I17" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J17" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1203,7 +1289,7 @@
     <row outlineLevel="0" r="18">
       <c r="A18" s="0" t="inlineStr">
         <is>
-          <t>ELEANORE CARELESS</t>
+          <t>JEAN KILGANNON</t>
         </is>
       </c>
       <c r="B18" s="0" t="inlineStr">
@@ -1213,22 +1299,22 @@
       </c>
       <c r="C18" s="0" t="inlineStr">
         <is>
-          <t>1899.79</t>
+          <t>48</t>
         </is>
       </c>
       <c r="D18" s="0" t="inlineStr">
         <is>
-          <t>6.1699999999999999</t>
+          <t>1121.6099999999999</t>
         </is>
       </c>
       <c r="E18" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3.9900000000000002</t>
         </is>
       </c>
       <c r="F18" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G18" s="0" t="inlineStr">
@@ -1242,6 +1328,11 @@
         </is>
       </c>
       <c r="I18" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J18" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1250,7 +1341,7 @@
     <row outlineLevel="0" r="19">
       <c r="A19" s="0" t="inlineStr">
         <is>
-          <t>ISSIAH LOB</t>
+          <t>DAMITA BAELDE</t>
         </is>
       </c>
       <c r="B19" s="0" t="inlineStr">
@@ -1260,22 +1351,22 @@
       </c>
       <c r="C19" s="0" t="inlineStr">
         <is>
-          <t>1923.3800000000001</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D19" s="0" t="inlineStr">
         <is>
-          <t>5.3600000000000003</t>
+          <t>1070.9200000000001</t>
         </is>
       </c>
       <c r="E19" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.05</t>
         </is>
       </c>
       <c r="F19" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G19" s="0" t="inlineStr">
@@ -1289,6 +1380,11 @@
         </is>
       </c>
       <c r="I19" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J19" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1297,32 +1393,32 @@
     <row outlineLevel="0" r="20">
       <c r="A20" s="0" t="inlineStr">
         <is>
-          <t>TREVER DU FRAY</t>
+          <t>HUGHIE MARVELL</t>
         </is>
       </c>
       <c r="B20" s="0" t="inlineStr">
         <is>
-          <t>Hombre</t>
+          <t>Mujer</t>
         </is>
       </c>
       <c r="C20" s="0" t="inlineStr">
         <is>
-          <t>1937.0599999999999</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D20" s="0" t="inlineStr">
         <is>
-          <t>6.7000000000000002</t>
+          <t>954.70000000000005</t>
         </is>
       </c>
       <c r="E20" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3.9399999999999999</t>
         </is>
       </c>
       <c r="F20" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G20" s="0" t="inlineStr">
@@ -1336,6 +1432,11 @@
         </is>
       </c>
       <c r="I20" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J20" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1344,7 +1445,7 @@
     <row outlineLevel="0" r="21">
       <c r="A21" s="0" t="inlineStr">
         <is>
-          <t>ISA WAYMAN</t>
+          <t>ERWIN FOXWELL</t>
         </is>
       </c>
       <c r="B21" s="0" t="inlineStr">
@@ -1354,22 +1455,22 @@
       </c>
       <c r="C21" s="0" t="inlineStr">
         <is>
-          <t>2415.1199999999999</t>
+          <t>54</t>
         </is>
       </c>
       <c r="D21" s="0" t="inlineStr">
         <is>
-          <t>5.4100000000000001</t>
+          <t>849.94000000000005</t>
         </is>
       </c>
       <c r="E21" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.2800000000000002</t>
         </is>
       </c>
       <c r="F21" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G21" s="0" t="inlineStr">
@@ -1383,6 +1484,11 @@
         </is>
       </c>
       <c r="I21" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J21" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1391,7 +1497,7 @@
     <row outlineLevel="0" r="22">
       <c r="A22" s="0" t="inlineStr">
         <is>
-          <t>JUNIE BLOWFIELD</t>
+          <t>NELLI JAKES</t>
         </is>
       </c>
       <c r="B22" s="0" t="inlineStr">
@@ -1401,22 +1507,22 @@
       </c>
       <c r="C22" s="0" t="inlineStr">
         <is>
-          <t>2448.2600000000002</t>
+          <t>59</t>
         </is>
       </c>
       <c r="D22" s="0" t="inlineStr">
         <is>
-          <t>4.0800000000000001</t>
+          <t>821.05999999999995</t>
         </is>
       </c>
       <c r="E22" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>5.1200000000000001</t>
         </is>
       </c>
       <c r="F22" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G22" s="0" t="inlineStr">
@@ -1430,6 +1536,11 @@
         </is>
       </c>
       <c r="I22" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J22" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1438,7 +1549,7 @@
     <row outlineLevel="0" r="23">
       <c r="A23" s="0" t="inlineStr">
         <is>
-          <t>RENADO DOBIE</t>
+          <t>PIP WILFINGER</t>
         </is>
       </c>
       <c r="B23" s="0" t="inlineStr">
@@ -1448,22 +1559,22 @@
       </c>
       <c r="C23" s="0" t="inlineStr">
         <is>
-          <t>2449.9400000000001</t>
+          <t>62</t>
         </is>
       </c>
       <c r="D23" s="0" t="inlineStr">
         <is>
-          <t>5.25</t>
+          <t>818.07000000000005</t>
         </is>
       </c>
       <c r="E23" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>4.6200000000000001</t>
         </is>
       </c>
       <c r="F23" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G23" s="0" t="inlineStr">
@@ -1477,6 +1588,11 @@
         </is>
       </c>
       <c r="I23" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J23" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1485,32 +1601,32 @@
     <row outlineLevel="0" r="24">
       <c r="A24" s="0" t="inlineStr">
         <is>
-          <t>CAREY BILLINGTON</t>
+          <t>TRIS DOCHON</t>
         </is>
       </c>
       <c r="B24" s="0" t="inlineStr">
         <is>
-          <t>Mujer</t>
+          <t>Hombre</t>
         </is>
       </c>
       <c r="C24" s="0" t="inlineStr">
         <is>
-          <t>2454.9400000000001</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D24" s="0" t="inlineStr">
         <is>
-          <t>3.27</t>
+          <t>817.49000000000001</t>
         </is>
       </c>
       <c r="E24" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>6.1100000000000003</t>
         </is>
       </c>
       <c r="F24" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G24" s="0" t="inlineStr">
@@ -1524,6 +1640,11 @@
         </is>
       </c>
       <c r="I24" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J24" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1532,32 +1653,32 @@
     <row outlineLevel="0" r="25">
       <c r="A25" s="0" t="inlineStr">
         <is>
-          <t>BEVVY CARRAGHER</t>
+          <t>MARCHELLE WITHROP</t>
         </is>
       </c>
       <c r="B25" s="0" t="inlineStr">
         <is>
-          <t>Hombre</t>
+          <t>Mujer</t>
         </is>
       </c>
       <c r="C25" s="0" t="inlineStr">
         <is>
-          <t>2875.3499999999999</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D25" s="0" t="inlineStr">
         <is>
-          <t>2.3399999999999999</t>
+          <t>663.26999999999998</t>
         </is>
       </c>
       <c r="E25" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.27</t>
         </is>
       </c>
       <c r="F25" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G25" s="0" t="inlineStr">
@@ -1571,6 +1692,11 @@
         </is>
       </c>
       <c r="I25" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J25" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1579,7 +1705,7 @@
     <row outlineLevel="0" r="26">
       <c r="A26" s="0" t="inlineStr">
         <is>
-          <t>ANSTICE DRACHE</t>
+          <t>DOROTEYA ROOKEBY</t>
         </is>
       </c>
       <c r="B26" s="0" t="inlineStr">
@@ -1589,22 +1715,22 @@
       </c>
       <c r="C26" s="0" t="inlineStr">
         <is>
-          <t>2916.96</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D26" s="0" t="inlineStr">
         <is>
-          <t>2.5699999999999998</t>
+          <t>597.66999999999996</t>
         </is>
       </c>
       <c r="E26" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>1.6100000000000001</t>
         </is>
       </c>
       <c r="F26" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G26" s="0" t="inlineStr">
@@ -1618,6 +1744,11 @@
         </is>
       </c>
       <c r="I26" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J26" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>
@@ -1626,7 +1757,7 @@
     <row outlineLevel="0" r="27">
       <c r="A27" s="0" t="inlineStr">
         <is>
-          <t>AME CRUM</t>
+          <t>JOBI MCINTEE</t>
         </is>
       </c>
       <c r="B27" s="0" t="inlineStr">
@@ -1636,22 +1767,22 @@
       </c>
       <c r="C27" s="0" t="inlineStr">
         <is>
-          <t>2999.1999999999998</t>
+          <t>33</t>
         </is>
       </c>
       <c r="D27" s="0" t="inlineStr">
         <is>
-          <t>3.2799999999999998</t>
+          <t>543.21000000000004</t>
         </is>
       </c>
       <c r="E27" s="0" t="inlineStr">
         <is>
-          <t>4</t>
+          <t>3.6499999999999999</t>
         </is>
       </c>
       <c r="F27" s="0" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>4</t>
         </is>
       </c>
       <c r="G27" s="0" t="inlineStr">
@@ -1665,6 +1796,11 @@
         </is>
       </c>
       <c r="I27" s="0" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
+      <c r="J27" s="0" t="inlineStr">
         <is>
           <t>SI</t>
         </is>

</xml_diff>